<commit_message>
Unpin all knapp och mer filterkontroll. ny data
</commit_message>
<xml_diff>
--- a/electron/backend/data/Testplan 2.0.xlsx
+++ b/electron/backend/data/Testplan 2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NASTS473A\Tirawa\Malin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SoftwareDev\Trafikverket projekt\Trafikverket-GIT\electron\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66A3A17B-D042-458D-AE02-9D83A7D83903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3442894E-F3A4-4C8C-BD67-75311329801C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1365" windowWidth="45525" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UT 2025" sheetId="7" r:id="rId1"/>
@@ -532,7 +532,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -586,9 +586,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -966,9 +963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049BB223-A6B5-4D3E-ACA7-4531434772CF}">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y50" sqref="Y50"/>
+      <selection pane="bottomLeft" activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,7 +1149,7 @@
       </c>
       <c r="X2" s="4">
         <f t="shared" ref="X2:X14" ca="1" si="5">TODAY()-W2</f>
-        <v>-32</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -1211,10 +1208,9 @@
       <c r="S3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="T3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="19"/>
       <c r="V3" s="18">
         <f t="shared" si="3"/>
         <v>45831</v>
@@ -1225,7 +1221,7 @@
       </c>
       <c r="X3" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-137</v>
+        <v>-120</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -1284,10 +1280,9 @@
       <c r="S4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="19">
+      <c r="T4" s="18">
         <v>45797</v>
       </c>
-      <c r="U4" s="19"/>
       <c r="V4" s="18">
         <f t="shared" si="3"/>
         <v>45722</v>
@@ -1298,7 +1293,7 @@
       </c>
       <c r="X4" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-28</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -1357,10 +1352,9 @@
       <c r="S5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="T5" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U5" s="19"/>
       <c r="V5" s="18">
         <f t="shared" si="3"/>
         <v>45829</v>
@@ -1371,7 +1365,7 @@
       </c>
       <c r="X5" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-135</v>
+        <v>-118</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -1430,10 +1424,9 @@
       <c r="S6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="19">
+      <c r="T6" s="18">
         <v>45797</v>
       </c>
-      <c r="U6" s="19"/>
       <c r="V6" s="18">
         <f t="shared" si="3"/>
         <v>45722</v>
@@ -1444,7 +1437,7 @@
       </c>
       <c r="X6" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-28</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -1503,10 +1496,9 @@
       <c r="S7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T7" s="19">
+      <c r="T7" s="18">
         <v>45898</v>
       </c>
-      <c r="U7" s="19"/>
       <c r="V7" s="18">
         <f t="shared" si="3"/>
         <v>45829</v>
@@ -1517,7 +1509,7 @@
       </c>
       <c r="X7" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-135</v>
+        <v>-118</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1576,10 +1568,9 @@
       <c r="S8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="19">
+      <c r="T8" s="18">
         <v>45797</v>
       </c>
-      <c r="U8" s="19"/>
       <c r="V8" s="18">
         <f t="shared" si="3"/>
         <v>45722</v>
@@ -1590,7 +1581,7 @@
       </c>
       <c r="X8" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-28</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -1649,10 +1640,9 @@
       <c r="S9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="19">
+      <c r="T9" s="18">
         <v>45898</v>
       </c>
-      <c r="U9" s="19"/>
       <c r="V9" s="18">
         <f t="shared" si="3"/>
         <v>45829</v>
@@ -1663,7 +1653,7 @@
       </c>
       <c r="X9" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-135</v>
+        <v>-118</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -1724,10 +1714,12 @@
       <c r="S10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="19">
+      <c r="T10" s="18">
         <v>45797</v>
       </c>
-      <c r="U10" s="19"/>
+      <c r="U10" s="18">
+        <v>45801</v>
+      </c>
       <c r="V10" s="18">
         <f t="shared" si="3"/>
         <v>45722</v>
@@ -1738,7 +1730,7 @@
       </c>
       <c r="X10" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-28</v>
+        <v>-11</v>
       </c>
       <c r="Y10" s="5" t="s">
         <v>25</v>
@@ -1802,10 +1794,9 @@
       <c r="S11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="19">
+      <c r="T11" s="18">
         <v>45898</v>
       </c>
-      <c r="U11" s="19"/>
       <c r="V11" s="18">
         <f t="shared" si="3"/>
         <v>45829</v>
@@ -1816,7 +1807,7 @@
       </c>
       <c r="X11" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-135</v>
+        <v>-118</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>25</v>
@@ -1880,10 +1871,9 @@
       <c r="S12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="19">
+      <c r="T12" s="18">
         <v>45898</v>
       </c>
-      <c r="U12" s="19"/>
       <c r="V12" s="18">
         <f t="shared" si="3"/>
         <v>45829</v>
@@ -1894,7 +1884,7 @@
       </c>
       <c r="X12" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-135</v>
+        <v>-118</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>25</v>
@@ -1947,7 +1937,7 @@
         <v>45417</v>
       </c>
       <c r="P13" s="18">
-        <f>O13+(365*M13)</f>
+        <f t="shared" ref="P13:P28" si="6">O13+(365*M13)</f>
         <v>45782</v>
       </c>
       <c r="Q13" s="18">
@@ -1956,10 +1946,10 @@
       <c r="S13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="19">
+      <c r="T13" s="18">
         <v>45801</v>
       </c>
-      <c r="U13" s="19">
+      <c r="U13" s="18">
         <v>45801</v>
       </c>
       <c r="V13" s="18">
@@ -1972,7 +1962,7 @@
       </c>
       <c r="X13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-28</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -2022,7 +2012,7 @@
         <v>45417</v>
       </c>
       <c r="P14" s="18">
-        <f>O14+(365*M14)</f>
+        <f t="shared" si="6"/>
         <v>45782</v>
       </c>
       <c r="Q14" s="18">
@@ -2031,10 +2021,9 @@
       <c r="S14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T14" s="19">
+      <c r="T14" s="18">
         <v>45801</v>
       </c>
-      <c r="U14" s="19"/>
       <c r="V14" s="18">
         <f t="shared" si="3"/>
         <v>45722</v>
@@ -2045,7 +2034,7 @@
       </c>
       <c r="X14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>-28</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -2068,7 +2057,7 @@
         <v>45</v>
       </c>
       <c r="G15" s="1" t="str">
-        <f>B15&amp;" - "&amp;C15&amp;" - "&amp;F15&amp;""</f>
+        <f t="shared" ref="G15:G56" si="7">B15&amp;" - "&amp;C15&amp;" - "&amp;F15&amp;""</f>
         <v>LDM - 218 - E (Hdn-Kls)</v>
       </c>
       <c r="H15" s="2">
@@ -2078,7 +2067,7 @@
         <v>299.61200000000002</v>
       </c>
       <c r="J15" s="2">
-        <f>I15-H15</f>
+        <f t="shared" ref="J15:J56" si="8">I15-H15</f>
         <v>14.581000000000017</v>
       </c>
       <c r="K15" s="3"/>
@@ -2092,11 +2081,11 @@
         <v>13</v>
       </c>
       <c r="O15" s="18">
-        <f>Q15</f>
+        <f t="shared" ref="O15:O23" si="9">Q15</f>
         <v>45437</v>
       </c>
       <c r="P15" s="18">
-        <f>O15+(365*M15)</f>
+        <f t="shared" si="6"/>
         <v>45802</v>
       </c>
       <c r="Q15" s="18">
@@ -2105,21 +2094,20 @@
       <c r="S15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="19">
+      <c r="T15" s="18">
         <v>45813</v>
       </c>
-      <c r="U15" s="19"/>
       <c r="V15" s="18">
-        <f>P15-60</f>
+        <f t="shared" ref="V15:V56" si="10">P15-60</f>
         <v>45742</v>
       </c>
       <c r="W15" s="18">
-        <f>P15+60</f>
+        <f t="shared" ref="W15:W56" si="11">P15+60</f>
         <v>45862</v>
       </c>
       <c r="X15" s="4">
-        <f ca="1">TODAY()-W15</f>
-        <v>-48</v>
+        <f t="shared" ref="X15:X56" ca="1" si="12">TODAY()-W15</f>
+        <v>-31</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -2142,7 +2130,7 @@
         <v>48</v>
       </c>
       <c r="G16" s="1" t="str">
-        <f>B16&amp;" - "&amp;C16&amp;" - "&amp;F16&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - E (Ob-Mog)</v>
       </c>
       <c r="H16" s="2">
@@ -2152,7 +2140,7 @@
         <v>262.86099999999999</v>
       </c>
       <c r="J16" s="2">
-        <f>I16-H16</f>
+        <f t="shared" si="8"/>
         <v>6.7099999999999795</v>
       </c>
       <c r="K16" s="3"/>
@@ -2166,11 +2154,11 @@
         <v>13</v>
       </c>
       <c r="O16" s="18">
-        <f>Q16</f>
+        <f t="shared" si="9"/>
         <v>45437</v>
       </c>
       <c r="P16" s="18">
-        <f>O16+(365*M16)</f>
+        <f t="shared" si="6"/>
         <v>45802</v>
       </c>
       <c r="Q16" s="18">
@@ -2179,21 +2167,20 @@
       <c r="S16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T16" s="19">
+      <c r="T16" s="18">
         <v>45813</v>
       </c>
-      <c r="U16" s="19"/>
       <c r="V16" s="18">
-        <f>P16-60</f>
+        <f t="shared" si="10"/>
         <v>45742</v>
       </c>
       <c r="W16" s="18">
-        <f>P16+60</f>
+        <f t="shared" si="11"/>
         <v>45862</v>
       </c>
       <c r="X16" s="4">
-        <f ca="1">TODAY()-W16</f>
-        <v>-48</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-31</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -2216,7 +2203,7 @@
         <v>49</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f>B17&amp;" - "&amp;C17&amp;" - "&amp;F17&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - E1 (Ob)</v>
       </c>
       <c r="H17" s="2">
@@ -2226,7 +2213,7 @@
         <v>38.491</v>
       </c>
       <c r="J17" s="2">
-        <f>I17-H17</f>
+        <f t="shared" si="8"/>
         <v>1.2160000000000011</v>
       </c>
       <c r="K17" s="3"/>
@@ -2240,11 +2227,11 @@
         <v>13</v>
       </c>
       <c r="O17" s="18">
-        <f>Q17</f>
+        <f t="shared" si="9"/>
         <v>45437</v>
       </c>
       <c r="P17" s="18">
-        <f>O17+(365*M17)</f>
+        <f t="shared" si="6"/>
         <v>45802</v>
       </c>
       <c r="Q17" s="18">
@@ -2253,21 +2240,20 @@
       <c r="S17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="19">
+      <c r="T17" s="18">
         <v>45829</v>
       </c>
-      <c r="U17" s="19"/>
       <c r="V17" s="18">
-        <f>P17-60</f>
+        <f t="shared" si="10"/>
         <v>45742</v>
       </c>
       <c r="W17" s="18">
-        <f>P17+60</f>
+        <f t="shared" si="11"/>
         <v>45862</v>
       </c>
       <c r="X17" s="4">
-        <f ca="1">TODAY()-W17</f>
-        <v>-48</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-31</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -2290,7 +2276,7 @@
         <v>50</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f>B18&amp;" - "&amp;C18&amp;" - "&amp;F18&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - E1 (Ob)(2a-1)</v>
       </c>
       <c r="H18" s="2">
@@ -2300,7 +2286,7 @@
         <v>257.21199999999999</v>
       </c>
       <c r="J18" s="2">
-        <f>I18-H18</f>
+        <f t="shared" si="8"/>
         <v>4.5000000000015916E-2</v>
       </c>
       <c r="K18" s="3"/>
@@ -2314,11 +2300,11 @@
         <v>13</v>
       </c>
       <c r="O18" s="18">
-        <f>Q18</f>
+        <f t="shared" si="9"/>
         <v>45437</v>
       </c>
       <c r="P18" s="18">
-        <f>O18+(365*M18)</f>
+        <f t="shared" si="6"/>
         <v>45802</v>
       </c>
       <c r="Q18" s="18">
@@ -2327,21 +2313,20 @@
       <c r="S18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="19">
+      <c r="T18" s="18">
         <v>45829</v>
       </c>
-      <c r="U18" s="19"/>
       <c r="V18" s="18">
-        <f>P18-60</f>
+        <f t="shared" si="10"/>
         <v>45742</v>
       </c>
       <c r="W18" s="18">
-        <f>P18+60</f>
+        <f t="shared" si="11"/>
         <v>45862</v>
       </c>
       <c r="X18" s="4">
-        <f ca="1">TODAY()-W18</f>
-        <v>-48</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-31</v>
       </c>
       <c r="Y18" s="5" t="s">
         <v>25</v>
@@ -2367,7 +2352,7 @@
         <v>51</v>
       </c>
       <c r="G19" s="1" t="str">
-        <f>B19&amp;" - "&amp;C19&amp;" - "&amp;F19&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - E1 (Ob)(2b-2a)</v>
       </c>
       <c r="H19" s="2">
@@ -2377,7 +2362,7 @@
         <v>38.615000000000002</v>
       </c>
       <c r="J19" s="2">
-        <f>I19-H19</f>
+        <f t="shared" si="8"/>
         <v>0.12400000000000233</v>
       </c>
       <c r="K19" s="3"/>
@@ -2391,11 +2376,11 @@
         <v>13</v>
       </c>
       <c r="O19" s="18">
-        <f>Q19</f>
+        <f t="shared" si="9"/>
         <v>45437</v>
       </c>
       <c r="P19" s="18">
-        <f>O19+(365*M19)</f>
+        <f t="shared" si="6"/>
         <v>45802</v>
       </c>
       <c r="Q19" s="18">
@@ -2404,21 +2389,20 @@
       <c r="S19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="19">
+      <c r="T19" s="18">
         <v>45829</v>
       </c>
-      <c r="U19" s="19"/>
       <c r="V19" s="18">
-        <f>P19-60</f>
+        <f t="shared" si="10"/>
         <v>45742</v>
       </c>
       <c r="W19" s="18">
-        <f>P19+60</f>
+        <f t="shared" si="11"/>
         <v>45862</v>
       </c>
       <c r="X19" s="4">
-        <f ca="1">TODAY()-W19</f>
-        <v>-48</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-31</v>
       </c>
       <c r="Y19" s="5" t="s">
         <v>25</v>
@@ -2444,7 +2428,7 @@
         <v>53</v>
       </c>
       <c r="G20" s="1" t="str">
-        <f>B20&amp;" - "&amp;C20&amp;" - "&amp;F20&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - N (Kls-Bn)</v>
       </c>
       <c r="H20" s="2">
@@ -2454,7 +2438,7 @@
         <v>316.25</v>
       </c>
       <c r="J20" s="2">
-        <f>I20-H20</f>
+        <f t="shared" si="8"/>
         <v>16.637999999999977</v>
       </c>
       <c r="K20" s="3"/>
@@ -2468,11 +2452,11 @@
         <v>13</v>
       </c>
       <c r="O20" s="18">
-        <f>Q20</f>
+        <f t="shared" si="9"/>
         <v>45437</v>
       </c>
       <c r="P20" s="18">
-        <f>O20+(365*M20)</f>
+        <f t="shared" si="6"/>
         <v>45802</v>
       </c>
       <c r="Q20" s="18">
@@ -2481,21 +2465,20 @@
       <c r="S20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="19">
+      <c r="T20" s="18">
         <v>45813</v>
       </c>
-      <c r="U20" s="19"/>
       <c r="V20" s="18">
-        <f>P20-60</f>
+        <f t="shared" si="10"/>
         <v>45742</v>
       </c>
       <c r="W20" s="18">
-        <f>P20+60</f>
+        <f t="shared" si="11"/>
         <v>45862</v>
       </c>
       <c r="X20" s="4">
-        <f ca="1">TODAY()-W20</f>
-        <v>-48</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-31</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -2518,7 +2501,7 @@
         <v>54</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f>B21&amp;" - "&amp;C21&amp;" - "&amp;F21&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - N (Mog-Hdn)</v>
       </c>
       <c r="H21" s="2">
@@ -2528,7 +2511,7 @@
         <v>285.03100000000001</v>
       </c>
       <c r="J21" s="2">
-        <f>I21-H21</f>
+        <f t="shared" si="8"/>
         <v>22.170000000000016</v>
       </c>
       <c r="K21" s="3"/>
@@ -2542,11 +2525,11 @@
         <v>13</v>
       </c>
       <c r="O21" s="18">
-        <f>Q21</f>
+        <f t="shared" si="9"/>
         <v>45437</v>
       </c>
       <c r="P21" s="18">
-        <f>O21+(365*M21)</f>
+        <f t="shared" si="6"/>
         <v>45802</v>
       </c>
       <c r="Q21" s="18">
@@ -2555,21 +2538,20 @@
       <c r="S21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T21" s="19">
+      <c r="T21" s="18">
         <v>45813</v>
       </c>
-      <c r="U21" s="19"/>
       <c r="V21" s="18">
-        <f>P21-60</f>
+        <f t="shared" si="10"/>
         <v>45742</v>
       </c>
       <c r="W21" s="18">
-        <f>P21+60</f>
+        <f t="shared" si="11"/>
         <v>45862</v>
       </c>
       <c r="X21" s="4">
-        <f ca="1">TODAY()-W21</f>
-        <v>-48</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-31</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -2592,7 +2574,7 @@
         <v>55</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f>B22&amp;" - "&amp;C22&amp;" - "&amp;F22&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - U (Kls-Bn)</v>
       </c>
       <c r="H22" s="2">
@@ -2602,7 +2584,7 @@
         <v>316.25</v>
       </c>
       <c r="J22" s="2">
-        <f>I22-H22</f>
+        <f t="shared" si="8"/>
         <v>16.637999999999977</v>
       </c>
       <c r="K22" s="3"/>
@@ -2616,11 +2598,11 @@
         <v>13</v>
       </c>
       <c r="O22" s="18">
-        <f>Q22</f>
+        <f t="shared" si="9"/>
         <v>45435</v>
       </c>
       <c r="P22" s="18">
-        <f>O22+(365*M22)</f>
+        <f t="shared" si="6"/>
         <v>45800</v>
       </c>
       <c r="Q22" s="18">
@@ -2629,21 +2611,20 @@
       <c r="S22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="19">
+      <c r="T22" s="18">
         <v>45826</v>
       </c>
-      <c r="U22" s="19"/>
       <c r="V22" s="18">
-        <f>P22-60</f>
+        <f t="shared" si="10"/>
         <v>45740</v>
       </c>
       <c r="W22" s="18">
-        <f>P22+60</f>
+        <f t="shared" si="11"/>
         <v>45860</v>
       </c>
       <c r="X22" s="4">
-        <f ca="1">TODAY()-W22</f>
-        <v>-46</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-29</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -2666,7 +2647,7 @@
         <v>56</v>
       </c>
       <c r="G23" s="1" t="str">
-        <f>B23&amp;" - "&amp;C23&amp;" - "&amp;F23&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 218 - U (Mog-Hdn)</v>
       </c>
       <c r="H23" s="2">
@@ -2676,7 +2657,7 @@
         <v>284.88099999999997</v>
       </c>
       <c r="J23" s="2">
-        <f>I23-H23</f>
+        <f t="shared" si="8"/>
         <v>22.019999999999982</v>
       </c>
       <c r="K23" s="3"/>
@@ -2690,11 +2671,11 @@
         <v>13</v>
       </c>
       <c r="O23" s="18">
-        <f>Q23</f>
+        <f t="shared" si="9"/>
         <v>45435</v>
       </c>
       <c r="P23" s="18">
-        <f>O23+(365*M23)</f>
+        <f t="shared" si="6"/>
         <v>45800</v>
       </c>
       <c r="Q23" s="18">
@@ -2703,21 +2684,20 @@
       <c r="S23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T23" s="19">
+      <c r="T23" s="18">
         <v>45826</v>
       </c>
-      <c r="U23" s="19"/>
       <c r="V23" s="18">
-        <f>P23-60</f>
+        <f t="shared" si="10"/>
         <v>45740</v>
       </c>
       <c r="W23" s="18">
-        <f>P23+60</f>
+        <f t="shared" si="11"/>
         <v>45860</v>
       </c>
       <c r="X23" s="4">
-        <f ca="1">TODAY()-W23</f>
-        <v>-46</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-29</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -2740,7 +2720,7 @@
         <v>59</v>
       </c>
       <c r="G24" s="1" t="str">
-        <f>B24&amp;" - "&amp;C24&amp;" - "&amp;F24&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 221 - E</v>
       </c>
       <c r="H24" s="2">
@@ -2750,7 +2730,7 @@
         <v>751.82500000000005</v>
       </c>
       <c r="J24" s="2">
-        <f>I24-H24</f>
+        <f t="shared" si="8"/>
         <v>164.54000000000008</v>
       </c>
       <c r="K24" s="3"/>
@@ -2767,27 +2747,26 @@
         <v>45068</v>
       </c>
       <c r="P24" s="18">
-        <f>O24+(365*M24)</f>
+        <f t="shared" si="6"/>
         <v>45798</v>
       </c>
       <c r="S24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T24" s="19">
+      <c r="T24" s="18">
         <v>45827</v>
       </c>
-      <c r="U24" s="19"/>
       <c r="V24" s="18">
-        <f>P24-60</f>
+        <f t="shared" si="10"/>
         <v>45738</v>
       </c>
       <c r="W24" s="18">
-        <f>P24+60</f>
+        <f t="shared" si="11"/>
         <v>45858</v>
       </c>
       <c r="X24" s="4">
-        <f ca="1">TODAY()-W24</f>
-        <v>-44</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-27</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -2810,7 +2789,7 @@
         <v>59</v>
       </c>
       <c r="G25" s="1" t="str">
-        <f>B25&amp;" - "&amp;C25&amp;" - "&amp;F25&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 222 - E</v>
       </c>
       <c r="H25" s="2">
@@ -2820,7 +2799,7 @@
         <v>587.28499999999997</v>
       </c>
       <c r="J25" s="2">
-        <f>I25-H25</f>
+        <f t="shared" si="8"/>
         <v>2.8159999999999172</v>
       </c>
       <c r="K25" s="3" t="s">
@@ -2840,7 +2819,7 @@
         <v>45431</v>
       </c>
       <c r="P25" s="18">
-        <f>O25+(365*M25)</f>
+        <f t="shared" si="6"/>
         <v>45796</v>
       </c>
       <c r="Q25" s="18">
@@ -2852,21 +2831,20 @@
       <c r="S25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="19">
+      <c r="T25" s="18">
         <v>45827</v>
       </c>
-      <c r="U25" s="19"/>
       <c r="V25" s="18">
-        <f>P25-60</f>
+        <f t="shared" si="10"/>
         <v>45736</v>
       </c>
       <c r="W25" s="18">
-        <f>P25+60</f>
+        <f t="shared" si="11"/>
         <v>45856</v>
       </c>
       <c r="X25" s="4">
-        <f ca="1">TODAY()-W25</f>
-        <v>-42</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-25</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -2889,7 +2867,7 @@
         <v>59</v>
       </c>
       <c r="G26" s="1" t="str">
-        <f>B26&amp;" - "&amp;C26&amp;" - "&amp;F26&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 222 - E</v>
       </c>
       <c r="H26" s="2">
@@ -2899,7 +2877,7 @@
         <v>586</v>
       </c>
       <c r="J26" s="2">
-        <f>I26-H26</f>
+        <f t="shared" si="8"/>
         <v>1.5309999999999491</v>
       </c>
       <c r="K26" s="3" t="s">
@@ -2918,7 +2896,7 @@
         <v>45534</v>
       </c>
       <c r="P26" s="18">
-        <f>O26+(365*M26)</f>
+        <f t="shared" si="6"/>
         <v>45899</v>
       </c>
       <c r="Q26" s="18">
@@ -2930,21 +2908,20 @@
       <c r="S26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T26" s="19" t="s">
+      <c r="T26" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U26" s="19"/>
       <c r="V26" s="18">
-        <f>P26-60</f>
+        <f t="shared" si="10"/>
         <v>45839</v>
       </c>
       <c r="W26" s="18">
-        <f>P26+60</f>
+        <f t="shared" si="11"/>
         <v>45959</v>
       </c>
       <c r="X26" s="4">
-        <f ca="1">TODAY()-W26</f>
-        <v>-145</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-128</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -2967,7 +2944,7 @@
         <v>59</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f>B27&amp;" - "&amp;C27&amp;" - "&amp;F27&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 223 - E</v>
       </c>
       <c r="H27" s="2">
@@ -2977,7 +2954,7 @@
         <v>584.46900000000005</v>
       </c>
       <c r="J27" s="2">
-        <f>I27-H27</f>
+        <f t="shared" si="8"/>
         <v>68.395000000000095</v>
       </c>
       <c r="K27" s="3" t="s">
@@ -2997,7 +2974,7 @@
         <v>45431</v>
       </c>
       <c r="P27" s="18">
-        <f>O27+(365*M27)</f>
+        <f t="shared" si="6"/>
         <v>45796</v>
       </c>
       <c r="Q27" s="18">
@@ -3009,21 +2986,20 @@
       <c r="S27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="19">
+      <c r="T27" s="18">
         <v>45828</v>
       </c>
-      <c r="U27" s="19"/>
       <c r="V27" s="18">
-        <f>P27-60</f>
+        <f t="shared" si="10"/>
         <v>45736</v>
       </c>
       <c r="W27" s="18">
-        <f>P27+60</f>
+        <f t="shared" si="11"/>
         <v>45856</v>
       </c>
       <c r="X27" s="4">
-        <f ca="1">TODAY()-W27</f>
-        <v>-42</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-25</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -3046,7 +3022,7 @@
         <v>59</v>
       </c>
       <c r="G28" s="1" t="str">
-        <f>B28&amp;" - "&amp;C28&amp;" - "&amp;F28&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDM - 223 - E</v>
       </c>
       <c r="H28" s="2">
@@ -3056,7 +3032,7 @@
         <v>584.46900000000005</v>
       </c>
       <c r="J28" s="2">
-        <f>I28-H28</f>
+        <f t="shared" si="8"/>
         <v>68.395000000000095</v>
       </c>
       <c r="K28" s="3" t="s">
@@ -3075,7 +3051,7 @@
         <v>45534</v>
       </c>
       <c r="P28" s="18">
-        <f>O28+(365*M28)</f>
+        <f t="shared" si="6"/>
         <v>45899</v>
       </c>
       <c r="Q28" s="18">
@@ -3087,21 +3063,20 @@
       <c r="S28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T28" s="19" t="s">
+      <c r="T28" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U28" s="19"/>
       <c r="V28" s="18">
-        <f>P28-60</f>
+        <f t="shared" si="10"/>
         <v>45839</v>
       </c>
       <c r="W28" s="18">
-        <f>P28+60</f>
+        <f t="shared" si="11"/>
         <v>45959</v>
       </c>
       <c r="X28" s="4">
-        <f ca="1">TODAY()-W28</f>
-        <v>-145</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-128</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -3124,7 +3099,7 @@
         <v>64</v>
       </c>
       <c r="G29" s="1" t="str">
-        <f>B29&amp;" - "&amp;C29&amp;" - "&amp;F29&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N2S</v>
       </c>
       <c r="H29" s="2">
@@ -3134,7 +3109,7 @@
         <v>11.7</v>
       </c>
       <c r="J29" s="2">
-        <f>I29-H29</f>
+        <f t="shared" si="8"/>
         <v>9.4059999999999988</v>
       </c>
       <c r="K29" s="3"/>
@@ -3152,7 +3127,7 @@
         <v>45366</v>
       </c>
       <c r="P29" s="18">
-        <f>O29+365</f>
+        <f t="shared" ref="P29:P42" si="13">O29+365</f>
         <v>45731</v>
       </c>
       <c r="Q29" s="18">
@@ -3164,23 +3139,23 @@
       <c r="S29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T29" s="19">
+      <c r="T29" s="18">
         <v>45759</v>
       </c>
-      <c r="U29" s="19">
+      <c r="U29" s="18">
         <v>45759</v>
       </c>
       <c r="V29" s="18">
-        <f>P29-60</f>
+        <f t="shared" si="10"/>
         <v>45671</v>
       </c>
       <c r="W29" s="18">
-        <f>P29+60</f>
+        <f t="shared" si="11"/>
         <v>45791</v>
       </c>
       <c r="X29" s="4">
-        <f ca="1">TODAY()-W29</f>
-        <v>23</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>40</v>
       </c>
       <c r="Y29" s="5" t="s">
         <v>65</v>
@@ -3206,7 +3181,7 @@
         <v>64</v>
       </c>
       <c r="G30" s="1" t="str">
-        <f>B30&amp;" - "&amp;C30&amp;" - "&amp;F30&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N2S</v>
       </c>
       <c r="H30" s="2">
@@ -3216,7 +3191,7 @@
         <v>11.7</v>
       </c>
       <c r="J30" s="2">
-        <f>I30-H30</f>
+        <f t="shared" si="8"/>
         <v>9.4059999999999988</v>
       </c>
       <c r="K30" s="3"/>
@@ -3234,7 +3209,7 @@
         <v>45563</v>
       </c>
       <c r="P30" s="18">
-        <f>O30+365</f>
+        <f t="shared" si="13"/>
         <v>45928</v>
       </c>
       <c r="Q30" s="18">
@@ -3246,21 +3221,20 @@
       <c r="S30" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="19">
+      <c r="T30" s="18">
         <v>45759</v>
       </c>
-      <c r="U30" s="19"/>
       <c r="V30" s="18">
-        <f>P30-60</f>
+        <f t="shared" si="10"/>
         <v>45868</v>
       </c>
       <c r="W30" s="18">
-        <f>P30+60</f>
+        <f t="shared" si="11"/>
         <v>45988</v>
       </c>
       <c r="X30" s="4">
-        <f ca="1">TODAY()-W30</f>
-        <v>-174</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-157</v>
       </c>
       <c r="Y30" s="5" t="s">
         <v>65</v>
@@ -3286,7 +3260,7 @@
         <v>68</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f>B31&amp;" - "&amp;C31&amp;" - "&amp;F31&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N3 (Cst-Tmö)</v>
       </c>
       <c r="H31" s="2">
@@ -3296,7 +3270,7 @@
         <v>4.1029999999999998</v>
       </c>
       <c r="J31" s="2">
-        <f>I31-H31</f>
+        <f t="shared" si="8"/>
         <v>4.1029999999999998</v>
       </c>
       <c r="K31" s="3"/>
@@ -3314,7 +3288,7 @@
         <v>45359</v>
       </c>
       <c r="P31" s="18">
-        <f>O31+365</f>
+        <f t="shared" si="13"/>
         <v>45724</v>
       </c>
       <c r="Q31" s="18">
@@ -3326,23 +3300,23 @@
       <c r="S31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T31" s="19">
+      <c r="T31" s="18">
         <v>45751</v>
       </c>
-      <c r="U31" s="19">
+      <c r="U31" s="18">
         <v>45751</v>
       </c>
       <c r="V31" s="18">
-        <f>P31-60</f>
+        <f t="shared" si="10"/>
         <v>45664</v>
       </c>
       <c r="W31" s="18">
-        <f>P31+60</f>
+        <f t="shared" si="11"/>
         <v>45784</v>
       </c>
       <c r="X31" s="4">
-        <f ca="1">TODAY()-W31</f>
-        <v>30</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>47</v>
       </c>
       <c r="Y31" s="5" t="s">
         <v>65</v>
@@ -3368,7 +3342,7 @@
         <v>68</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f>B32&amp;" - "&amp;C32&amp;" - "&amp;F32&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N3 (Cst-Tmö)</v>
       </c>
       <c r="H32" s="2">
@@ -3378,7 +3352,7 @@
         <v>4.1029999999999998</v>
       </c>
       <c r="J32" s="2">
-        <f>I32-H32</f>
+        <f t="shared" si="8"/>
         <v>4.1029999999999998</v>
       </c>
       <c r="K32" s="3"/>
@@ -3396,7 +3370,7 @@
         <v>45562</v>
       </c>
       <c r="P32" s="18">
-        <f>O32+365</f>
+        <f t="shared" si="13"/>
         <v>45927</v>
       </c>
       <c r="Q32" s="18">
@@ -3408,21 +3382,20 @@
       <c r="S32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T32" s="19" t="s">
+      <c r="T32" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U32" s="19"/>
       <c r="V32" s="18">
-        <f>P32-60</f>
+        <f t="shared" si="10"/>
         <v>45867</v>
       </c>
       <c r="W32" s="18">
-        <f>P32+60</f>
+        <f t="shared" si="11"/>
         <v>45987</v>
       </c>
       <c r="X32" s="4">
-        <f ca="1">TODAY()-W32</f>
-        <v>-173</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-156</v>
       </c>
       <c r="Y32" s="5" t="s">
         <v>65</v>
@@ -3448,7 +3421,7 @@
         <v>69</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f>B33&amp;" - "&amp;C33&amp;" - "&amp;F33&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N3S</v>
       </c>
       <c r="H33" s="2">
@@ -3458,7 +3431,7 @@
         <v>8.5489999999999995</v>
       </c>
       <c r="J33" s="2">
-        <f>I33-H33</f>
+        <f t="shared" si="8"/>
         <v>1.4859999999999998</v>
       </c>
       <c r="K33" s="3"/>
@@ -3476,7 +3449,7 @@
         <v>45395</v>
       </c>
       <c r="P33" s="18">
-        <f>O33+365</f>
+        <f t="shared" si="13"/>
         <v>45760</v>
       </c>
       <c r="Q33" s="18">
@@ -3488,23 +3461,23 @@
       <c r="S33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T33" s="19">
+      <c r="T33" s="18">
         <v>45760</v>
       </c>
-      <c r="U33" s="19">
+      <c r="U33" s="18">
         <v>45760</v>
       </c>
       <c r="V33" s="18">
-        <f>P33-60</f>
+        <f t="shared" si="10"/>
         <v>45700</v>
       </c>
       <c r="W33" s="18">
-        <f>P33+60</f>
+        <f t="shared" si="11"/>
         <v>45820</v>
       </c>
       <c r="X33" s="4">
-        <f ca="1">TODAY()-W33</f>
-        <v>-6</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>11</v>
       </c>
       <c r="Y33" s="5" t="s">
         <v>65</v>
@@ -3530,7 +3503,7 @@
         <v>69</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f>B34&amp;" - "&amp;C34&amp;" - "&amp;F34&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N3S</v>
       </c>
       <c r="H34" s="2">
@@ -3540,7 +3513,7 @@
         <v>8.5489999999999995</v>
       </c>
       <c r="J34" s="2">
-        <f>I34-H34</f>
+        <f t="shared" si="8"/>
         <v>1.4859999999999998</v>
       </c>
       <c r="K34" s="3"/>
@@ -3558,7 +3531,7 @@
         <v>45577</v>
       </c>
       <c r="P34" s="18">
-        <f>O34+365</f>
+        <f t="shared" si="13"/>
         <v>45942</v>
       </c>
       <c r="Q34" s="18">
@@ -3570,21 +3543,20 @@
       <c r="S34" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T34" s="19" t="s">
+      <c r="T34" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U34" s="19"/>
       <c r="V34" s="18">
-        <f>P34-60</f>
+        <f t="shared" si="10"/>
         <v>45882</v>
       </c>
       <c r="W34" s="18">
-        <f>P34+60</f>
+        <f t="shared" si="11"/>
         <v>46002</v>
       </c>
       <c r="X34" s="4">
-        <f ca="1">TODAY()-W34</f>
-        <v>-188</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-171</v>
       </c>
       <c r="Y34" s="5" t="s">
         <v>65</v>
@@ -3610,7 +3582,7 @@
         <v>70</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f>B35&amp;" - "&amp;C35&amp;" - "&amp;F35&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N4</v>
       </c>
       <c r="H35" s="2">
@@ -3620,7 +3592,7 @@
         <v>4.1029999999999998</v>
       </c>
       <c r="J35" s="2">
-        <f>I35-H35</f>
+        <f t="shared" si="8"/>
         <v>0.81699999999999973</v>
       </c>
       <c r="K35" s="3"/>
@@ -3638,7 +3610,7 @@
         <v>45465</v>
       </c>
       <c r="P35" s="18">
-        <f>O35+365</f>
+        <f t="shared" si="13"/>
         <v>45830</v>
       </c>
       <c r="Q35" s="18">
@@ -3650,21 +3622,20 @@
       <c r="S35" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T35" s="19">
+      <c r="T35" s="18">
         <v>45846</v>
       </c>
-      <c r="U35" s="19"/>
       <c r="V35" s="18">
-        <f>P35-60</f>
+        <f t="shared" si="10"/>
         <v>45770</v>
       </c>
       <c r="W35" s="18">
-        <f>P35+60</f>
+        <f t="shared" si="11"/>
         <v>45890</v>
       </c>
       <c r="X35" s="4">
-        <f ca="1">TODAY()-W35</f>
-        <v>-76</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-59</v>
       </c>
       <c r="Y35" s="5" t="s">
         <v>65</v>
@@ -3690,7 +3661,7 @@
         <v>70</v>
       </c>
       <c r="G36" s="1" t="str">
-        <f>B36&amp;" - "&amp;C36&amp;" - "&amp;F36&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N4</v>
       </c>
       <c r="H36" s="2">
@@ -3700,7 +3671,7 @@
         <v>4.1029999999999998</v>
       </c>
       <c r="J36" s="2">
-        <f>I36-H36</f>
+        <f t="shared" si="8"/>
         <v>0.81699999999999973</v>
       </c>
       <c r="K36" s="3"/>
@@ -3718,7 +3689,7 @@
         <v>45562</v>
       </c>
       <c r="P36" s="18">
-        <f>O36+365</f>
+        <f t="shared" si="13"/>
         <v>45927</v>
       </c>
       <c r="Q36" s="18">
@@ -3730,21 +3701,20 @@
       <c r="S36" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T36" s="19" t="s">
+      <c r="T36" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="U36" s="19"/>
       <c r="V36" s="18">
-        <f>P36-60</f>
+        <f t="shared" si="10"/>
         <v>45867</v>
       </c>
       <c r="W36" s="18">
-        <f>P36+60</f>
+        <f t="shared" si="11"/>
         <v>45987</v>
       </c>
       <c r="X36" s="4">
-        <f ca="1">TODAY()-W36</f>
-        <v>-173</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-156</v>
       </c>
       <c r="Y36" s="5" t="s">
         <v>65</v>
@@ -3770,7 +3740,7 @@
         <v>71</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f>B37&amp;" - "&amp;C37&amp;" - "&amp;F37&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N5</v>
       </c>
       <c r="H37" s="2">
@@ -3780,7 +3750,7 @@
         <v>4.0469999999999997</v>
       </c>
       <c r="J37" s="2">
-        <f>I37-H37</f>
+        <f t="shared" si="8"/>
         <v>0.7629999999999999</v>
       </c>
       <c r="K37" s="3"/>
@@ -3798,7 +3768,7 @@
         <v>45367</v>
       </c>
       <c r="P37" s="18">
-        <f>O37+365</f>
+        <f t="shared" si="13"/>
         <v>45732</v>
       </c>
       <c r="Q37" s="18">
@@ -3810,23 +3780,23 @@
       <c r="S37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T37" s="19">
+      <c r="T37" s="18">
         <v>45752</v>
       </c>
-      <c r="U37" s="19">
+      <c r="U37" s="18">
         <v>45752</v>
       </c>
       <c r="V37" s="18">
-        <f>P37-60</f>
+        <f t="shared" si="10"/>
         <v>45672</v>
       </c>
       <c r="W37" s="18">
-        <f>P37+60</f>
+        <f t="shared" si="11"/>
         <v>45792</v>
       </c>
       <c r="X37" s="4">
-        <f ca="1">TODAY()-W37</f>
-        <v>22</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>39</v>
       </c>
       <c r="Y37" s="5" t="s">
         <v>65</v>
@@ -3852,7 +3822,7 @@
         <v>71</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f>B38&amp;" - "&amp;C38&amp;" - "&amp;F38&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - N5</v>
       </c>
       <c r="H38" s="2">
@@ -3862,7 +3832,7 @@
         <v>4.0469999999999997</v>
       </c>
       <c r="J38" s="2">
-        <f>I38-H38</f>
+        <f t="shared" si="8"/>
         <v>0.7629999999999999</v>
       </c>
       <c r="K38" s="3"/>
@@ -3880,7 +3850,7 @@
         <v>45562</v>
       </c>
       <c r="P38" s="18">
-        <f>O38+365</f>
+        <f t="shared" si="13"/>
         <v>45927</v>
       </c>
       <c r="Q38" s="18">
@@ -3892,21 +3862,20 @@
       <c r="S38" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T38" s="19">
+      <c r="T38" s="18">
         <v>45752</v>
       </c>
-      <c r="U38" s="19"/>
       <c r="V38" s="18">
-        <f>P38-60</f>
+        <f t="shared" si="10"/>
         <v>45867</v>
       </c>
       <c r="W38" s="18">
-        <f>P38+60</f>
+        <f t="shared" si="11"/>
         <v>45987</v>
       </c>
       <c r="X38" s="4">
-        <f ca="1">TODAY()-W38</f>
-        <v>-173</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-156</v>
       </c>
       <c r="Y38" s="5" t="s">
         <v>65</v>
@@ -3932,7 +3901,7 @@
         <v>72</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f>B39&amp;" - "&amp;C39&amp;" - "&amp;F39&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - NS (Äs)(97b-konn8)</v>
       </c>
       <c r="H39" s="2">
@@ -3942,7 +3911,7 @@
         <v>8.8450000000000006</v>
       </c>
       <c r="J39" s="2">
-        <f>I39-H39</f>
+        <f t="shared" si="8"/>
         <v>0.29600000000000115</v>
       </c>
       <c r="K39" s="3"/>
@@ -3960,7 +3929,7 @@
         <v>45395</v>
       </c>
       <c r="P39" s="18">
-        <f>O39+365</f>
+        <f t="shared" si="13"/>
         <v>45760</v>
       </c>
       <c r="Q39" s="18">
@@ -3972,23 +3941,23 @@
       <c r="S39" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T39" s="19">
+      <c r="T39" s="18">
         <v>45759</v>
       </c>
-      <c r="U39" s="19">
+      <c r="U39" s="18">
         <v>45760</v>
       </c>
       <c r="V39" s="18">
-        <f>P39-60</f>
+        <f t="shared" si="10"/>
         <v>45700</v>
       </c>
       <c r="W39" s="18">
-        <f>P39+60</f>
+        <f t="shared" si="11"/>
         <v>45820</v>
       </c>
       <c r="X39" s="4">
-        <f ca="1">TODAY()-W39</f>
-        <v>-6</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>11</v>
       </c>
       <c r="Y39" s="5" t="s">
         <v>65</v>
@@ -4014,7 +3983,7 @@
         <v>72</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f>B40&amp;" - "&amp;C40&amp;" - "&amp;F40&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - NS (Äs)(97b-konn8)</v>
       </c>
       <c r="H40" s="2">
@@ -4024,7 +3993,7 @@
         <v>8.8450000000000006</v>
       </c>
       <c r="J40" s="2">
-        <f>I40-H40</f>
+        <f t="shared" si="8"/>
         <v>0.29600000000000115</v>
       </c>
       <c r="K40" s="3"/>
@@ -4042,7 +4011,7 @@
         <v>45577</v>
       </c>
       <c r="P40" s="18">
-        <f>O40+365</f>
+        <f t="shared" si="13"/>
         <v>45942</v>
       </c>
       <c r="Q40" s="18">
@@ -4054,21 +4023,20 @@
       <c r="S40" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T40" s="19">
+      <c r="T40" s="18">
         <v>45759</v>
       </c>
-      <c r="U40" s="19"/>
       <c r="V40" s="18">
-        <f>P40-60</f>
+        <f t="shared" si="10"/>
         <v>45882</v>
       </c>
       <c r="W40" s="18">
-        <f>P40+60</f>
+        <f t="shared" si="11"/>
         <v>46002</v>
       </c>
       <c r="X40" s="4">
-        <f ca="1">TODAY()-W40</f>
-        <v>-188</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-171</v>
       </c>
       <c r="Y40" s="5" t="s">
         <v>65</v>
@@ -4094,7 +4062,7 @@
         <v>73</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f>B41&amp;" - "&amp;C41&amp;" - "&amp;F41&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - NS (Äs)(konn8-gr02)</v>
       </c>
       <c r="H41" s="2">
@@ -4104,7 +4072,7 @@
         <v>55</v>
       </c>
       <c r="J41" s="2">
-        <f>I41-H41</f>
+        <f t="shared" si="8"/>
         <v>4.2999999999999261E-2</v>
       </c>
       <c r="K41" s="3"/>
@@ -4122,7 +4090,7 @@
         <v>45395</v>
       </c>
       <c r="P41" s="18">
-        <f>O41+365</f>
+        <f t="shared" si="13"/>
         <v>45760</v>
       </c>
       <c r="Q41" s="18">
@@ -4134,23 +4102,23 @@
       <c r="S41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T41" s="19">
+      <c r="T41" s="18">
         <v>45759</v>
       </c>
-      <c r="U41" s="19">
+      <c r="U41" s="18">
         <v>45760</v>
       </c>
       <c r="V41" s="18">
-        <f>P41-60</f>
+        <f t="shared" si="10"/>
         <v>45700</v>
       </c>
       <c r="W41" s="18">
-        <f>P41+60</f>
+        <f t="shared" si="11"/>
         <v>45820</v>
       </c>
       <c r="X41" s="4">
-        <f ca="1">TODAY()-W41</f>
-        <v>-6</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>11</v>
       </c>
       <c r="Y41" s="5" t="s">
         <v>65</v>
@@ -4176,7 +4144,7 @@
         <v>73</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f>B42&amp;" - "&amp;C42&amp;" - "&amp;F42&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 401 - NS (Äs)(konn8-gr02)</v>
       </c>
       <c r="H42" s="2">
@@ -4186,7 +4154,7 @@
         <v>55</v>
       </c>
       <c r="J42" s="2">
-        <f>I42-H42</f>
+        <f t="shared" si="8"/>
         <v>4.2999999999999261E-2</v>
       </c>
       <c r="K42" s="3"/>
@@ -4204,7 +4172,7 @@
         <v>45577</v>
       </c>
       <c r="P42" s="18">
-        <f>O42+365</f>
+        <f t="shared" si="13"/>
         <v>45942</v>
       </c>
       <c r="Q42" s="18">
@@ -4216,21 +4184,20 @@
       <c r="S42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T42" s="19">
+      <c r="T42" s="18">
         <v>45759</v>
       </c>
-      <c r="U42" s="19"/>
       <c r="V42" s="18">
-        <f>P42-60</f>
+        <f t="shared" si="10"/>
         <v>45882</v>
       </c>
       <c r="W42" s="18">
-        <f>P42+60</f>
+        <f t="shared" si="11"/>
         <v>46002</v>
       </c>
       <c r="X42" s="4">
-        <f ca="1">TODAY()-W42</f>
-        <v>-188</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-171</v>
       </c>
       <c r="Y42" s="5" t="s">
         <v>65</v>
@@ -4256,7 +4223,7 @@
         <v>59</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f>B43&amp;" - "&amp;C43&amp;" - "&amp;F43&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 831 - E</v>
       </c>
       <c r="H43" s="2">
@@ -4266,7 +4233,7 @@
         <v>20.010000000000002</v>
       </c>
       <c r="J43" s="2">
-        <f>I43-H43</f>
+        <f t="shared" si="8"/>
         <v>17.154000000000003</v>
       </c>
       <c r="K43" s="3" t="s">
@@ -4282,11 +4249,11 @@
         <v>21</v>
       </c>
       <c r="O43" s="18">
-        <f>Q43</f>
+        <f t="shared" ref="O43:O49" si="14">Q43</f>
         <v>45571</v>
       </c>
       <c r="P43" s="18">
-        <f>O43+(365*M43)</f>
+        <f t="shared" ref="P43:P56" si="15">O43+(365*M43)</f>
         <v>45936</v>
       </c>
       <c r="Q43" s="18">
@@ -4295,21 +4262,20 @@
       <c r="S43" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T43" s="19">
+      <c r="T43" s="18">
         <v>45773</v>
       </c>
-      <c r="U43" s="19"/>
       <c r="V43" s="18">
-        <f>P43-60</f>
+        <f t="shared" si="10"/>
         <v>45876</v>
       </c>
       <c r="W43" s="18">
-        <f>P43+60</f>
+        <f t="shared" si="11"/>
         <v>45996</v>
       </c>
       <c r="X43" s="4">
-        <f ca="1">TODAY()-W43</f>
-        <v>-182</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-165</v>
       </c>
       <c r="Y43" s="5" t="s">
         <v>25</v>
@@ -4335,7 +4301,7 @@
         <v>59</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f>B44&amp;" - "&amp;C44&amp;" - "&amp;F44&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 832 - E</v>
       </c>
       <c r="H44" s="2">
@@ -4345,7 +4311,7 @@
         <v>120.705</v>
       </c>
       <c r="J44" s="2">
-        <f>I44-H44</f>
+        <f t="shared" si="8"/>
         <v>38.143000000000001</v>
       </c>
       <c r="K44" s="3"/>
@@ -4359,11 +4325,11 @@
         <v>13</v>
       </c>
       <c r="O44" s="18">
-        <f>Q44</f>
+        <f t="shared" si="14"/>
         <v>45382</v>
       </c>
       <c r="P44" s="18">
-        <f>O44+(365*M44)</f>
+        <f t="shared" si="15"/>
         <v>45747</v>
       </c>
       <c r="Q44" s="18">
@@ -4372,23 +4338,23 @@
       <c r="S44" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T44" s="19">
+      <c r="T44" s="18">
         <v>45774</v>
       </c>
-      <c r="U44" s="19">
+      <c r="U44" s="18">
         <v>45774</v>
       </c>
       <c r="V44" s="18">
-        <f>P44-60</f>
+        <f t="shared" si="10"/>
         <v>45687</v>
       </c>
       <c r="W44" s="18">
-        <f>P44+60</f>
+        <f t="shared" si="11"/>
         <v>45807</v>
       </c>
       <c r="X44" s="4">
-        <f ca="1">TODAY()-W44</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>24</v>
       </c>
       <c r="Y44" s="5" t="s">
         <v>25</v>
@@ -4414,7 +4380,7 @@
         <v>78</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f>B45&amp;" - "&amp;C45&amp;" - "&amp;F45&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 832 - E1 (Bg)(23b-24b)</v>
       </c>
       <c r="H45" s="2">
@@ -4424,7 +4390,7 @@
         <v>120.389</v>
       </c>
       <c r="J45" s="2">
-        <f>I45-H45</f>
+        <f t="shared" si="8"/>
         <v>0.22699999999998965</v>
       </c>
       <c r="K45" s="3"/>
@@ -4438,11 +4404,11 @@
         <v>13</v>
       </c>
       <c r="O45" s="18">
-        <f>Q45</f>
+        <f t="shared" si="14"/>
         <v>45380</v>
       </c>
       <c r="P45" s="18">
-        <f>O45+(365*M45)</f>
+        <f t="shared" si="15"/>
         <v>45745</v>
       </c>
       <c r="Q45" s="18">
@@ -4451,23 +4417,23 @@
       <c r="S45" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T45" s="19">
+      <c r="T45" s="18">
         <v>45774</v>
       </c>
-      <c r="U45" s="19">
+      <c r="U45" s="18">
         <v>45773</v>
       </c>
       <c r="V45" s="18">
-        <f>P45-60</f>
+        <f t="shared" si="10"/>
         <v>45685</v>
       </c>
       <c r="W45" s="18">
-        <f>P45+60</f>
+        <f t="shared" si="11"/>
         <v>45805</v>
       </c>
       <c r="X45" s="4">
-        <f ca="1">TODAY()-W45</f>
-        <v>9</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>26</v>
       </c>
       <c r="Y45" s="5" t="s">
         <v>79</v>
@@ -4493,7 +4459,7 @@
         <v>80</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f>B46&amp;" - "&amp;C46&amp;" - "&amp;F46&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 832 - E1 (Bg)(gr03-23b)</v>
       </c>
       <c r="H46" s="2">
@@ -4503,7 +4469,7 @@
         <v>76.677999999999997</v>
       </c>
       <c r="J46" s="2">
-        <f>I46-H46</f>
+        <f t="shared" si="8"/>
         <v>0.28300000000000125</v>
       </c>
       <c r="K46" s="3"/>
@@ -4517,11 +4483,11 @@
         <v>13</v>
       </c>
       <c r="O46" s="18">
-        <f>Q46</f>
+        <f t="shared" si="14"/>
         <v>45380</v>
       </c>
       <c r="P46" s="18">
-        <f>O46+(365*M46)</f>
+        <f t="shared" si="15"/>
         <v>45745</v>
       </c>
       <c r="Q46" s="18">
@@ -4530,23 +4496,23 @@
       <c r="S46" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T46" s="19">
+      <c r="T46" s="18">
         <v>45774</v>
       </c>
-      <c r="U46" s="19">
+      <c r="U46" s="18">
         <v>45773</v>
       </c>
       <c r="V46" s="18">
-        <f>P46-60</f>
+        <f t="shared" si="10"/>
         <v>45685</v>
       </c>
       <c r="W46" s="18">
-        <f>P46+60</f>
+        <f t="shared" si="11"/>
         <v>45805</v>
       </c>
       <c r="X46" s="4">
-        <f ca="1">TODAY()-W46</f>
-        <v>9</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>26</v>
       </c>
       <c r="Y46" s="5" t="s">
         <v>79</v>
@@ -4572,7 +4538,7 @@
         <v>81</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f>B47&amp;" - "&amp;C47&amp;" - "&amp;F47&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 832 - E1 (Hf)</v>
       </c>
       <c r="H47" s="2">
@@ -4582,7 +4548,7 @@
         <v>122.84399999999999</v>
       </c>
       <c r="J47" s="2">
-        <f>I47-H47</f>
+        <f t="shared" si="8"/>
         <v>1.1099999999999994</v>
       </c>
       <c r="K47" s="3"/>
@@ -4596,11 +4562,11 @@
         <v>13</v>
       </c>
       <c r="O47" s="18">
-        <f>Q47</f>
+        <f t="shared" si="14"/>
         <v>45384</v>
       </c>
       <c r="P47" s="18">
-        <f>O47+(365*M47)</f>
+        <f t="shared" si="15"/>
         <v>45749</v>
       </c>
       <c r="Q47" s="18">
@@ -4609,23 +4575,23 @@
       <c r="S47" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T47" s="19">
+      <c r="T47" s="18">
         <v>45774</v>
       </c>
-      <c r="U47" s="19">
+      <c r="U47" s="18">
         <v>45776</v>
       </c>
       <c r="V47" s="18">
-        <f>P47-60</f>
+        <f t="shared" si="10"/>
         <v>45689</v>
       </c>
       <c r="W47" s="18">
-        <f>P47+60</f>
+        <f t="shared" si="11"/>
         <v>45809</v>
       </c>
       <c r="X47" s="4">
-        <f ca="1">TODAY()-W47</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>22</v>
       </c>
       <c r="Y47" s="5" t="s">
         <v>79</v>
@@ -4651,7 +4617,7 @@
         <v>59</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f>B48&amp;" - "&amp;C48&amp;" - "&amp;F48&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 833 - E</v>
       </c>
       <c r="H48" s="2">
@@ -4661,7 +4627,7 @@
         <v>148.464</v>
       </c>
       <c r="J48" s="2">
-        <f>I48-H48</f>
+        <f t="shared" si="8"/>
         <v>27.759</v>
       </c>
       <c r="K48" s="3"/>
@@ -4675,11 +4641,11 @@
         <v>13</v>
       </c>
       <c r="O48" s="18">
-        <f>Q48</f>
+        <f t="shared" si="14"/>
         <v>45381</v>
       </c>
       <c r="P48" s="18">
-        <f>O48+(365*M48)</f>
+        <f t="shared" si="15"/>
         <v>45746</v>
       </c>
       <c r="Q48" s="18">
@@ -4688,23 +4654,23 @@
       <c r="S48" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T48" s="19">
+      <c r="T48" s="18">
         <v>45774</v>
       </c>
-      <c r="U48" s="19">
+      <c r="U48" s="18">
         <v>45774</v>
       </c>
       <c r="V48" s="18">
-        <f>P48-60</f>
+        <f t="shared" si="10"/>
         <v>45686</v>
       </c>
       <c r="W48" s="18">
-        <f>P48+60</f>
+        <f t="shared" si="11"/>
         <v>45806</v>
       </c>
       <c r="X48" s="4">
-        <f ca="1">TODAY()-W48</f>
-        <v>8</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>25</v>
       </c>
       <c r="Y48" s="5" t="s">
         <v>25</v>
@@ -4730,7 +4696,7 @@
         <v>59</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f>B49&amp;" - "&amp;C49&amp;" - "&amp;F49&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDÖ - 841 - E</v>
       </c>
       <c r="H49" s="2">
@@ -4740,7 +4706,7 @@
         <v>121.73399999999999</v>
       </c>
       <c r="J49" s="2">
-        <f>I49-H49</f>
+        <f t="shared" si="8"/>
         <v>100.88199999999999</v>
       </c>
       <c r="K49" s="3"/>
@@ -4754,11 +4720,11 @@
         <v>13</v>
       </c>
       <c r="O49" s="18">
-        <f>Q49</f>
+        <f t="shared" si="14"/>
         <v>45384</v>
       </c>
       <c r="P49" s="18">
-        <f>O49+(365*M49)</f>
+        <f t="shared" si="15"/>
         <v>45749</v>
       </c>
       <c r="Q49" s="18">
@@ -4767,23 +4733,23 @@
       <c r="S49" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T49" s="19">
+      <c r="T49" s="18">
         <v>45776</v>
       </c>
-      <c r="U49" s="19">
+      <c r="U49" s="18">
         <v>45776</v>
       </c>
       <c r="V49" s="18">
-        <f>P49-60</f>
+        <f t="shared" si="10"/>
         <v>45689</v>
       </c>
       <c r="W49" s="18">
-        <f>P49+60</f>
+        <f t="shared" si="11"/>
         <v>45809</v>
       </c>
       <c r="X49" s="4">
-        <f ca="1">TODAY()-W49</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>22</v>
       </c>
       <c r="Y49" s="5" t="s">
         <v>25</v>
@@ -4809,7 +4775,7 @@
         <v>85</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f>B50&amp;" - "&amp;C50&amp;" - "&amp;F50&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 904 - N (Hb)</v>
       </c>
       <c r="H50" s="2">
@@ -4819,7 +4785,7 @@
         <v>244.761</v>
       </c>
       <c r="J50" s="2">
-        <f>I50-H50</f>
+        <f t="shared" si="8"/>
         <v>0.22999999999998977</v>
       </c>
       <c r="K50" s="3" t="s">
@@ -4838,7 +4804,7 @@
         <v>45591</v>
       </c>
       <c r="P50" s="18">
-        <f>O50+(365*M50)</f>
+        <f t="shared" si="15"/>
         <v>45956</v>
       </c>
       <c r="Q50" s="18">
@@ -4847,21 +4813,20 @@
       <c r="S50" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T50" s="19">
+      <c r="T50" s="18">
         <v>45765</v>
       </c>
-      <c r="U50" s="19"/>
       <c r="V50" s="18">
-        <f>P50-60</f>
+        <f t="shared" si="10"/>
         <v>45896</v>
       </c>
       <c r="W50" s="18">
-        <f>P50+60</f>
+        <f t="shared" si="11"/>
         <v>46016</v>
       </c>
       <c r="X50" s="4">
-        <f ca="1">TODAY()-W50</f>
-        <v>-202</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-185</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
@@ -4884,7 +4849,7 @@
         <v>87</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f>B51&amp;" - "&amp;C51&amp;" - "&amp;F51&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 904 - N (Hb-Hbgb)</v>
       </c>
       <c r="H51" s="2">
@@ -4894,7 +4859,7 @@
         <v>3.794</v>
       </c>
       <c r="J51" s="2">
-        <f>I51-H51</f>
+        <f t="shared" si="8"/>
         <v>2.8839999999999999</v>
       </c>
       <c r="K51" s="3"/>
@@ -4912,7 +4877,7 @@
         <v>45372</v>
       </c>
       <c r="P51" s="18">
-        <f>O51+(365*M51)</f>
+        <f t="shared" si="15"/>
         <v>45737</v>
       </c>
       <c r="Q51" s="18">
@@ -4921,23 +4886,23 @@
       <c r="S51" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T51" s="19">
+      <c r="T51" s="18">
         <v>45765</v>
       </c>
-      <c r="U51" s="19">
+      <c r="U51" s="18">
         <v>45766</v>
       </c>
       <c r="V51" s="18">
-        <f>P51-60</f>
+        <f t="shared" si="10"/>
         <v>45677</v>
       </c>
       <c r="W51" s="18">
-        <f>P51+60</f>
+        <f t="shared" si="11"/>
         <v>45797</v>
       </c>
       <c r="X51" s="4">
-        <f ca="1">TODAY()-W51</f>
-        <v>17</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
@@ -4960,7 +4925,7 @@
         <v>88</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f>B52&amp;" - "&amp;C52&amp;" - "&amp;F52&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 904 - U (Hb)</v>
       </c>
       <c r="H52" s="2">
@@ -4970,7 +4935,7 @@
         <v>244.809</v>
       </c>
       <c r="J52" s="2">
-        <f>I52-H52</f>
+        <f t="shared" si="8"/>
         <v>0.42799999999999727</v>
       </c>
       <c r="K52" s="3" t="s">
@@ -4990,7 +4955,7 @@
         <v>45372</v>
       </c>
       <c r="P52" s="18">
-        <f>O52+(365*M52)</f>
+        <f t="shared" si="15"/>
         <v>45737</v>
       </c>
       <c r="Q52" s="18">
@@ -4999,23 +4964,23 @@
       <c r="S52" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T52" s="19">
+      <c r="T52" s="18">
         <v>45765</v>
       </c>
-      <c r="U52" s="19">
+      <c r="U52" s="18">
         <v>45765</v>
       </c>
       <c r="V52" s="18">
-        <f>P52-60</f>
+        <f t="shared" si="10"/>
         <v>45677</v>
       </c>
       <c r="W52" s="18">
-        <f>P52+60</f>
+        <f t="shared" si="11"/>
         <v>45797</v>
       </c>
       <c r="X52" s="4">
-        <f ca="1">TODAY()-W52</f>
-        <v>17</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
@@ -5038,7 +5003,7 @@
         <v>88</v>
       </c>
       <c r="G53" s="1" t="str">
-        <f>B53&amp;" - "&amp;C53&amp;" - "&amp;F53&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 904 - U (Hb)</v>
       </c>
       <c r="H53" s="2">
@@ -5048,7 +5013,7 @@
         <v>244.809</v>
       </c>
       <c r="J53" s="2">
-        <f>I53-H53</f>
+        <f t="shared" si="8"/>
         <v>0.35699999999999932</v>
       </c>
       <c r="K53" s="3" t="s">
@@ -5067,7 +5032,7 @@
         <v>45591</v>
       </c>
       <c r="P53" s="18">
-        <f>O53+(365*M53)</f>
+        <f t="shared" si="15"/>
         <v>45956</v>
       </c>
       <c r="Q53" s="18">
@@ -5076,21 +5041,20 @@
       <c r="S53" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T53" s="19">
+      <c r="T53" s="18">
         <v>45765</v>
       </c>
-      <c r="U53" s="19"/>
       <c r="V53" s="18">
-        <f>P53-60</f>
+        <f t="shared" si="10"/>
         <v>45896</v>
       </c>
       <c r="W53" s="18">
-        <f>P53+60</f>
+        <f t="shared" si="11"/>
         <v>46016</v>
       </c>
       <c r="X53" s="4">
-        <f ca="1">TODAY()-W53</f>
-        <v>-202</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-185</v>
       </c>
       <c r="Z53" s="5" t="s">
         <v>89</v>
@@ -5116,7 +5080,7 @@
         <v>90</v>
       </c>
       <c r="G54" s="1" t="str">
-        <f>B54&amp;" - "&amp;C54&amp;" - "&amp;F54&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 904 - U (Hb-Hbgb)</v>
       </c>
       <c r="H54" s="2">
@@ -5126,7 +5090,7 @@
         <v>3.794</v>
       </c>
       <c r="J54" s="2">
-        <f>I54-H54</f>
+        <f t="shared" si="8"/>
         <v>2.8839999999999999</v>
       </c>
       <c r="K54" s="3"/>
@@ -5144,7 +5108,7 @@
         <v>45372</v>
       </c>
       <c r="P54" s="18">
-        <f>O54+(365*M54)</f>
+        <f t="shared" si="15"/>
         <v>45737</v>
       </c>
       <c r="Q54" s="18">
@@ -5153,23 +5117,23 @@
       <c r="S54" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T54" s="19">
+      <c r="T54" s="18">
         <v>45765</v>
       </c>
-      <c r="U54" s="19">
+      <c r="U54" s="18">
         <v>45765</v>
       </c>
       <c r="V54" s="18">
-        <f>P54-60</f>
+        <f t="shared" si="10"/>
         <v>45677</v>
       </c>
       <c r="W54" s="18">
-        <f>P54+60</f>
+        <f t="shared" si="11"/>
         <v>45797</v>
       </c>
       <c r="X54" s="4">
-        <f ca="1">TODAY()-W54</f>
-        <v>17</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
@@ -5192,7 +5156,7 @@
         <v>92</v>
       </c>
       <c r="G55" s="1" t="str">
-        <f>B55&amp;" - "&amp;C55&amp;" - "&amp;F55&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 909 - E (Hm)(553-gr03)</v>
       </c>
       <c r="H55" s="2">
@@ -5202,7 +5166,7 @@
         <v>0.90700000000000003</v>
       </c>
       <c r="J55" s="2">
-        <f>I55-H55</f>
+        <f t="shared" si="8"/>
         <v>0.33400000000000007</v>
       </c>
       <c r="K55" s="3"/>
@@ -5219,27 +5183,26 @@
         <v>45253</v>
       </c>
       <c r="P55" s="18">
-        <f>O55+(365*M55)</f>
+        <f t="shared" si="15"/>
         <v>45983</v>
       </c>
       <c r="S55" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T55" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="U55" s="19"/>
+      <c r="T55" s="18" t="s">
+        <v>22</v>
+      </c>
       <c r="V55" s="18">
-        <f>P55-60</f>
+        <f t="shared" si="10"/>
         <v>45923</v>
       </c>
       <c r="W55" s="18">
-        <f>P55+60</f>
+        <f t="shared" si="11"/>
         <v>46043</v>
       </c>
       <c r="X55" s="4">
-        <f ca="1">TODAY()-W55</f>
-        <v>-229</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-212</v>
       </c>
       <c r="Z55" s="5" t="s">
         <v>93</v>
@@ -5265,7 +5228,7 @@
         <v>94</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f>B56&amp;" - "&amp;C56&amp;" - "&amp;F56&amp;""</f>
+        <f t="shared" si="7"/>
         <v>LDS - 909 - E (Hm)(gr07-456))</v>
       </c>
       <c r="H56" s="2">
@@ -5275,7 +5238,7 @@
         <v>71.484999999999999</v>
       </c>
       <c r="J56" s="2">
-        <f>I56-H56</f>
+        <f t="shared" si="8"/>
         <v>0.49500000000000455</v>
       </c>
       <c r="K56" s="3"/>
@@ -5292,27 +5255,26 @@
         <v>45244</v>
       </c>
       <c r="P56" s="18">
-        <f>O56+(365*M56)</f>
+        <f t="shared" si="15"/>
         <v>45974</v>
       </c>
       <c r="S56" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T56" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="U56" s="19"/>
+      <c r="T56" s="18" t="s">
+        <v>22</v>
+      </c>
       <c r="V56" s="18">
-        <f>P56-60</f>
+        <f t="shared" si="10"/>
         <v>45914</v>
       </c>
       <c r="W56" s="18">
-        <f>P56+60</f>
+        <f t="shared" si="11"/>
         <v>46034</v>
       </c>
       <c r="X56" s="4">
-        <f ca="1">TODAY()-W56</f>
-        <v>-220</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>